<commit_message>
fix: Config Server connection in production - deutsche Übersetzungen funktionieren jetzt
- useConfig.ts: Use relative URL in production (via Nginx proxy)
- nginx.conf: Add /api/config/ proxy to config-server:8888
- Fixes: Frontend couldn't reach Config Server → i18n files not created
- Auto-registration now works as designed!

[CONFIG_HOOK_FIX_001]

🤖 Generated with Claude Code
Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/arbeitszeit.xlsx
+++ b/arbeitszeit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\morit\IdeaProjects\Eckert Enterprise\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84DC840D-D9B8-420B-BB1F-27845FEA6025}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C5032FA-3488-4152-98E7-F9B117C1BB7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A3DE9C98-0436-4FB4-B06B-7A93EE6B3D59}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="29">
   <si>
     <t>Arbeitsstunden Becker Moritz</t>
   </si>
@@ -120,6 +120,9 @@
   </si>
   <si>
     <t>18:00 - 24:00</t>
+  </si>
+  <si>
+    <t>17:00 - 24:00</t>
   </si>
 </sst>
 </file>
@@ -584,16 +587,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -932,8 +935,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE89B172-B3F2-4C47-A3CE-42F89B6F8F05}">
   <dimension ref="B1:F60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="I44" sqref="I44"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="I43" sqref="I43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1318,15 +1321,15 @@
       </c>
     </row>
     <row r="29" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="36">
+      <c r="B29" s="34">
         <v>14</v>
       </c>
-      <c r="C29" s="37"/>
-      <c r="D29" s="34">
+      <c r="C29" s="35"/>
+      <c r="D29" s="36">
         <f>D4+D5+D6+D7+D8+D10+D11+D12+D13+D14+D16+D17+D18+D19+D20+D22+D24+D23+D26+D25</f>
         <v>106.5</v>
       </c>
-      <c r="E29" s="35"/>
+      <c r="E29" s="37"/>
       <c r="F29" s="25">
         <f>B29*D29</f>
         <v>1491</v>
@@ -1418,9 +1421,11 @@
         <v>45953</v>
       </c>
       <c r="D38" s="6">
-        <v>0</v>
-      </c>
-      <c r="E38" s="6"/>
+        <v>7</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>28</v>
+      </c>
       <c r="F38" s="17"/>
     </row>
     <row r="39" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1699,32 +1704,32 @@
       </c>
     </row>
     <row r="60" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B60" s="36">
+      <c r="B60" s="34">
         <v>14</v>
       </c>
-      <c r="C60" s="37"/>
-      <c r="D60" s="34">
+      <c r="C60" s="35"/>
+      <c r="D60" s="36">
         <f>D35+D36+D37+D38+D39+D41+D42+D43+D44+D45+D47+D48+D49+D50+D51+D53+D55+D54+D57+D56</f>
-        <v>16.329999999999998</v>
-      </c>
-      <c r="E60" s="35"/>
+        <v>23.33</v>
+      </c>
+      <c r="E60" s="37"/>
       <c r="F60" s="25">
         <f>B60*D60</f>
-        <v>228.61999999999998</v>
+        <v>326.62</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B29:C29"/>
     <mergeCell ref="B33:F33"/>
     <mergeCell ref="B59:C59"/>
     <mergeCell ref="D59:E59"/>
     <mergeCell ref="B60:C60"/>
     <mergeCell ref="D60:E60"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B29:C29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
feat(frontend): add TrustedBy component with animated logo scroller
- TrustedBy component with two-row infinite scroll (LTR + RTL)
- 20 company logos copied from old project
- Black/White design with grayscale effect (color on hover)
- Pause animation on hover with smooth gradient masks
- Added scroll animations to Tailwind (animate-scroll-ltr/rtl)
- Integrated into Homepage after Hero section
- Config API v2.0: trustedBy.title key
- Updated frontend/CHANGELOG.md and root CHANGELOG.md
- Version bump: v2.16.0 → v2.17.0

[FRONTEND_TRUSTED_001]
[FRONTEND_ANIM_007]
[FRONTEND_PAGE_011]

🤖 Generated with Claude Code
Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/arbeitszeit.xlsx
+++ b/arbeitszeit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\morit\IdeaProjects\Eckert Enterprise\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C5032FA-3488-4152-98E7-F9B117C1BB7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A51160E-34F2-4D98-AA1D-8FA04A50BACC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A3DE9C98-0436-4FB4-B06B-7A93EE6B3D59}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="31">
   <si>
     <t>Arbeitsstunden Becker Moritz</t>
   </si>
@@ -123,6 +123,12 @@
   </si>
   <si>
     <t>17:00 - 24:00</t>
+  </si>
+  <si>
+    <t>18:30 - 24:00</t>
+  </si>
+  <si>
+    <t>18:00-24:00</t>
   </si>
 </sst>
 </file>
@@ -587,16 +593,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -936,7 +942,7 @@
   <dimension ref="B1:F60"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="I43" sqref="I43"/>
+      <selection activeCell="F55" sqref="F55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1321,15 +1327,15 @@
       </c>
     </row>
     <row r="29" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="34">
+      <c r="B29" s="36">
         <v>14</v>
       </c>
-      <c r="C29" s="35"/>
-      <c r="D29" s="36">
+      <c r="C29" s="37"/>
+      <c r="D29" s="34">
         <f>D4+D5+D6+D7+D8+D10+D11+D12+D13+D14+D16+D17+D18+D19+D20+D22+D24+D23+D26+D25</f>
         <v>106.5</v>
       </c>
-      <c r="E29" s="37"/>
+      <c r="E29" s="35"/>
       <c r="F29" s="25">
         <f>B29*D29</f>
         <v>1491</v>
@@ -1456,10 +1462,10 @@
         <v>45957</v>
       </c>
       <c r="D41" s="5">
-        <v>0</v>
+        <v>4.5</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="F41" s="26"/>
     </row>
@@ -1471,10 +1477,10 @@
         <v>45958</v>
       </c>
       <c r="D42" s="6">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E42" s="6" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="F42" s="27"/>
     </row>
@@ -1486,10 +1492,10 @@
         <v>45959</v>
       </c>
       <c r="D43" s="6">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E43" s="6" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="F43" s="27"/>
     </row>
@@ -1501,10 +1507,10 @@
         <v>45960</v>
       </c>
       <c r="D44" s="6">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E44" s="6" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="F44" s="27"/>
     </row>
@@ -1704,32 +1710,32 @@
       </c>
     </row>
     <row r="60" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B60" s="34">
+      <c r="B60" s="36">
         <v>14</v>
       </c>
-      <c r="C60" s="35"/>
-      <c r="D60" s="36">
+      <c r="C60" s="37"/>
+      <c r="D60" s="34">
         <f>D35+D36+D37+D38+D39+D41+D42+D43+D44+D45+D47+D48+D49+D50+D51+D53+D55+D54+D57+D56</f>
-        <v>23.33</v>
-      </c>
-      <c r="E60" s="37"/>
+        <v>42.83</v>
+      </c>
+      <c r="E60" s="35"/>
       <c r="F60" s="25">
         <f>B60*D60</f>
-        <v>326.62</v>
+        <v>599.62</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B33:F33"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="D59:E59"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="D60:E60"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="D28:E28"/>
     <mergeCell ref="D29:E29"/>
     <mergeCell ref="B28:C28"/>
     <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B33:F33"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="D59:E59"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="D60:E60"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fix: Design updates and documentation cleanup
- Fix bg-gray-50 to bg-white in PeterEckertSection (design guidelines)
- Update RaketenStart 4-Phasen to professional English formulations
- Update WissenschaftlicheFundierung conclusion (remove defensive language)
- Clean design for FinnlandQuellen page
- Update documentation versions
- Add nul to gitignore (Windows reserved filename)

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/arbeitszeit.xlsx
+++ b/arbeitszeit.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\morit\IdeaProjects\Eckert Enterprise\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A51160E-34F2-4D98-AA1D-8FA04A50BACC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58894D26-36A2-4863-9967-927C25953241}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A3DE9C98-0436-4FB4-B06B-7A93EE6B3D59}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A3DE9C98-0436-4FB4-B06B-7A93EE6B3D59}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="38">
   <si>
     <t>Arbeitsstunden Becker Moritz</t>
   </si>
@@ -129,6 +129,27 @@
   </si>
   <si>
     <t>18:00-24:00</t>
+  </si>
+  <si>
+    <t>18:00 - 22:00</t>
+  </si>
+  <si>
+    <t>18:00 - 23:00</t>
+  </si>
+  <si>
+    <t>18:00 - 22:30</t>
+  </si>
+  <si>
+    <t>18:00 - 01:00</t>
+  </si>
+  <si>
+    <t>Sam &amp; Son</t>
+  </si>
+  <si>
+    <t>1 &amp; 2</t>
+  </si>
+  <si>
+    <t>18 - 20 &amp; 14  - 20</t>
   </si>
 </sst>
 </file>
@@ -502,7 +523,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -593,16 +614,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -939,10 +963,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE89B172-B3F2-4C47-A3CE-42F89B6F8F05}">
-  <dimension ref="B1:F60"/>
+  <dimension ref="B1:F90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="F55" sqref="F55"/>
+    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="J49" sqref="J49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1327,15 +1351,15 @@
       </c>
     </row>
     <row r="29" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="36">
+      <c r="B29" s="34">
         <v>14</v>
       </c>
-      <c r="C29" s="37"/>
-      <c r="D29" s="34">
+      <c r="C29" s="35"/>
+      <c r="D29" s="36">
         <f>D4+D5+D6+D7+D8+D10+D11+D12+D13+D14+D16+D17+D18+D19+D20+D22+D24+D23+D26+D25</f>
         <v>106.5</v>
       </c>
-      <c r="E29" s="35"/>
+      <c r="E29" s="37"/>
       <c r="F29" s="25">
         <f>B29*D29</f>
         <v>1491</v>
@@ -1530,10 +1554,18 @@
       <c r="F45" s="28"/>
     </row>
     <row r="46" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="14"/>
-      <c r="C46" s="4"/>
-      <c r="D46" s="4"/>
-      <c r="E46" s="4"/>
+      <c r="B46" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C46" s="38" t="s">
+        <v>36</v>
+      </c>
+      <c r="D46" s="4">
+        <v>8</v>
+      </c>
+      <c r="E46" s="4" t="s">
+        <v>37</v>
+      </c>
       <c r="F46" s="3"/>
     </row>
     <row r="47" spans="2:6" x14ac:dyDescent="0.25">
@@ -1544,10 +1576,10 @@
         <v>45964</v>
       </c>
       <c r="D47" s="5">
-        <v>0</v>
-      </c>
-      <c r="E47" s="5" t="s">
-        <v>18</v>
+        <v>6</v>
+      </c>
+      <c r="E47" s="6" t="s">
+        <v>34</v>
       </c>
       <c r="F47" s="16"/>
     </row>
@@ -1559,10 +1591,10 @@
         <v>45965</v>
       </c>
       <c r="D48" s="6">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E48" s="6" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="F48" s="17"/>
     </row>
@@ -1574,10 +1606,10 @@
         <v>45966</v>
       </c>
       <c r="D49" s="6">
-        <v>0</v>
+        <v>4.5</v>
       </c>
       <c r="E49" s="6" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="F49" s="17"/>
     </row>
@@ -1589,10 +1621,10 @@
         <v>45967</v>
       </c>
       <c r="D50" s="6">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E50" s="6" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="F50" s="17"/>
     </row>
@@ -1626,7 +1658,7 @@
         <v>45971</v>
       </c>
       <c r="D53" s="19">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E53" s="5" t="s">
         <v>19</v>
@@ -1641,7 +1673,7 @@
         <v>45972</v>
       </c>
       <c r="D54" s="20">
-        <v>0</v>
+        <v>4.5</v>
       </c>
       <c r="E54" s="6" t="s">
         <v>11</v>
@@ -1656,10 +1688,10 @@
         <v>45973</v>
       </c>
       <c r="D55" s="20">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E55" s="6" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="F55" s="17"/>
     </row>
@@ -1671,7 +1703,7 @@
         <v>45974</v>
       </c>
       <c r="D56" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E56" s="6" t="s">
         <v>24</v>
@@ -1710,33 +1742,338 @@
       </c>
     </row>
     <row r="60" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B60" s="36">
+      <c r="B60" s="34">
         <v>14</v>
       </c>
-      <c r="C60" s="37"/>
-      <c r="D60" s="34">
-        <f>D35+D36+D37+D38+D39+D41+D42+D43+D44+D45+D47+D48+D49+D50+D51+D53+D55+D54+D57+D56</f>
-        <v>42.83</v>
-      </c>
-      <c r="E60" s="35"/>
+      <c r="C60" s="35"/>
+      <c r="D60" s="36">
+        <f>D35+D36+D37+D38+D39+D41+D42+D43+D44+D45+D47+D48+D49+D50+D51+D53+D55+D54+D57+D56+D46</f>
+        <v>84.83</v>
+      </c>
+      <c r="E60" s="37"/>
       <c r="F60" s="25">
         <f>B60*D60</f>
-        <v>599.62</v>
+        <v>1187.6199999999999</v>
+      </c>
+    </row>
+    <row r="62" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="63" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B63" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="C63" s="30"/>
+      <c r="D63" s="30"/>
+      <c r="E63" s="30"/>
+      <c r="F63" s="31"/>
+    </row>
+    <row r="64" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B64" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C64" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D64" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E64" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F64" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="65" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B65" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C65" s="10">
+        <v>45978</v>
+      </c>
+      <c r="D65" s="5"/>
+      <c r="E65" s="5"/>
+      <c r="F65" s="16"/>
+    </row>
+    <row r="66" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B66" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C66" s="8">
+        <v>45979</v>
+      </c>
+      <c r="D66" s="6"/>
+      <c r="E66" s="6"/>
+      <c r="F66" s="17"/>
+    </row>
+    <row r="67" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B67" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C67" s="8">
+        <v>45980</v>
+      </c>
+      <c r="D67" s="6"/>
+      <c r="E67" s="6"/>
+      <c r="F67" s="17"/>
+    </row>
+    <row r="68" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B68" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C68" s="8">
+        <v>45981</v>
+      </c>
+      <c r="D68" s="6"/>
+      <c r="E68" s="6"/>
+      <c r="F68" s="17"/>
+    </row>
+    <row r="69" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B69" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C69" s="9">
+        <v>45982</v>
+      </c>
+      <c r="D69" s="7"/>
+      <c r="E69" s="7"/>
+      <c r="F69" s="18"/>
+    </row>
+    <row r="70" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B70" s="14"/>
+      <c r="C70" s="4"/>
+      <c r="D70" s="4"/>
+      <c r="E70" s="4"/>
+      <c r="F70" s="3"/>
+    </row>
+    <row r="71" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B71" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C71" s="10">
+        <v>45985</v>
+      </c>
+      <c r="D71" s="5"/>
+      <c r="E71" s="5"/>
+      <c r="F71" s="26"/>
+    </row>
+    <row r="72" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B72" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C72" s="8">
+        <v>45986</v>
+      </c>
+      <c r="D72" s="6"/>
+      <c r="E72" s="6"/>
+      <c r="F72" s="27"/>
+    </row>
+    <row r="73" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B73" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C73" s="8">
+        <v>45987</v>
+      </c>
+      <c r="D73" s="6"/>
+      <c r="E73" s="6"/>
+      <c r="F73" s="27"/>
+    </row>
+    <row r="74" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B74" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C74" s="8">
+        <v>45988</v>
+      </c>
+      <c r="D74" s="6"/>
+      <c r="E74" s="6"/>
+      <c r="F74" s="27"/>
+    </row>
+    <row r="75" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B75" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C75" s="9">
+        <v>45989</v>
+      </c>
+      <c r="D75" s="7"/>
+      <c r="E75" s="7"/>
+      <c r="F75" s="28"/>
+    </row>
+    <row r="76" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B76" s="14"/>
+      <c r="C76" s="4"/>
+      <c r="D76" s="4"/>
+      <c r="E76" s="4"/>
+      <c r="F76" s="3"/>
+    </row>
+    <row r="77" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B77" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C77" s="22">
+        <v>45992</v>
+      </c>
+      <c r="D77" s="5"/>
+      <c r="E77" s="5"/>
+      <c r="F77" s="16"/>
+    </row>
+    <row r="78" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B78" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C78" s="23">
+        <v>45993</v>
+      </c>
+      <c r="D78" s="6"/>
+      <c r="E78" s="6"/>
+      <c r="F78" s="17"/>
+    </row>
+    <row r="79" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B79" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C79" s="23">
+        <v>45994</v>
+      </c>
+      <c r="D79" s="6"/>
+      <c r="E79" s="6"/>
+      <c r="F79" s="17"/>
+    </row>
+    <row r="80" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B80" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C80" s="23">
+        <v>45995</v>
+      </c>
+      <c r="D80" s="6"/>
+      <c r="E80" s="6"/>
+      <c r="F80" s="17"/>
+    </row>
+    <row r="81" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B81" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C81" s="24">
+        <v>45996</v>
+      </c>
+      <c r="D81" s="7"/>
+      <c r="E81" s="7"/>
+      <c r="F81" s="18"/>
+    </row>
+    <row r="82" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B82" s="14"/>
+      <c r="C82" s="4"/>
+      <c r="D82" s="4"/>
+      <c r="E82" s="4"/>
+      <c r="F82" s="3"/>
+    </row>
+    <row r="83" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B83" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C83" s="22">
+        <v>45971</v>
+      </c>
+      <c r="D83" s="19"/>
+      <c r="E83" s="5"/>
+      <c r="F83" s="16"/>
+    </row>
+    <row r="84" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B84" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C84" s="23">
+        <v>45972</v>
+      </c>
+      <c r="D84" s="20"/>
+      <c r="E84" s="6"/>
+      <c r="F84" s="17"/>
+    </row>
+    <row r="85" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B85" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C85" s="23">
+        <v>45973</v>
+      </c>
+      <c r="D85" s="20"/>
+      <c r="E85" s="6"/>
+      <c r="F85" s="17"/>
+    </row>
+    <row r="86" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B86" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C86" s="23">
+        <v>45974</v>
+      </c>
+      <c r="D86" s="20"/>
+      <c r="E86" s="6"/>
+      <c r="F86" s="17"/>
+    </row>
+    <row r="87" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B87" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C87" s="24">
+        <v>45975</v>
+      </c>
+      <c r="D87" s="21"/>
+      <c r="E87" s="7"/>
+      <c r="F87" s="18"/>
+    </row>
+    <row r="88" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B88" s="1"/>
+    </row>
+    <row r="89" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B89" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="C89" s="33"/>
+      <c r="D89" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="E89" s="33"/>
+      <c r="F89" s="13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="90" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B90" s="34">
+        <v>14</v>
+      </c>
+      <c r="C90" s="35"/>
+      <c r="D90" s="36">
+        <f>D65+D66+D67+D68+D69+D71+D72+D73+D74+D75+D77+D78+D79+D80+D81+D83+D85+D84+D87+D86</f>
+        <v>0</v>
+      </c>
+      <c r="E90" s="37"/>
+      <c r="F90" s="25">
+        <f>B90*D90</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="15">
+    <mergeCell ref="B63:F63"/>
+    <mergeCell ref="B89:C89"/>
+    <mergeCell ref="D89:E89"/>
+    <mergeCell ref="B90:C90"/>
+    <mergeCell ref="D90:E90"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B29:C29"/>
     <mergeCell ref="B33:F33"/>
     <mergeCell ref="B59:C59"/>
     <mergeCell ref="D59:E59"/>
     <mergeCell ref="B60:C60"/>
     <mergeCell ref="D60:E60"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B29:C29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>